<commit_message>
BOM Update with recommended FPGA version
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -89,9 +89,6 @@
     <t>http://www.digikey.de/short/3v93nm</t>
   </si>
   <si>
-    <t>10CL006YE144C8G</t>
-  </si>
-  <si>
     <t>DESCRIPTION</t>
   </si>
   <si>
@@ -110,21 +107,12 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>Cyclone 10 LP FPGA, 6k LE</t>
-  </si>
-  <si>
     <t>EQFP144</t>
   </si>
   <si>
     <t>can be replaced with other FPGAs on demand (see Schematic file)</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Intel/10CL006YE144C8G/</t>
-  </si>
-  <si>
-    <t>http://www.digikey.de/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=234870402</t>
-  </si>
-  <si>
     <t>Video DAC 8bit, 3Ch.</t>
   </si>
   <si>
@@ -143,9 +131,6 @@
     <t>Non-Inv Buffer 3Ch.</t>
   </si>
   <si>
-    <t>TI: DCT Package Footprint</t>
-  </si>
-  <si>
     <t>8-LSSOP, 8-MSOP</t>
   </si>
   <si>
@@ -501,6 +486,21 @@
   </si>
   <si>
     <t xml:space="preserve">IC FLASH 16MBIT 108MHZ 8SOIC </t>
+  </si>
+  <si>
+    <t>TI: DCT Package Footprint, Alternative: 74HC3G34DP</t>
+  </si>
+  <si>
+    <t>10CL010YE144C8G</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/en/altera/10CL010YE144I7G/544-3376-ND/7347620</t>
+  </si>
+  <si>
+    <t>http://www.mouser.de/ProductDetail/Intel/10CL010YE144C8G/</t>
+  </si>
+  <si>
+    <t>Cyclone 10 LP FPGA, 10k LE</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1347,22 +1347,22 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
-      </c>
-      <c r="I1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1370,25 +1370,25 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1396,25 +1396,25 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1428,16 +1428,16 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1451,151 +1451,151 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="I8" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -1604,50 +1604,50 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E11" t="s">
+      <c r="I11" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -1656,19 +1656,19 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1682,19 +1682,19 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1708,62 +1708,62 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1771,25 +1771,25 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
       <c r="D18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E18" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" t="s">
-        <v>79</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1797,106 +1797,106 @@
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F19" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="I19" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F22" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="I22" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1910,103 +1910,103 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F24" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F26" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2022,7 +2022,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId1" display="http://www.digikey.de/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=234870402"/>
     <hyperlink ref="I2" r:id="rId2"/>
     <hyperlink ref="H3" r:id="rId3"/>
     <hyperlink ref="I3" r:id="rId4"/>

</xml_diff>

<commit_message>
PCB Update: - unused VREF to VCCIO (see connection guideline) - unused DEV_CLRn and DEV_OE to GND (see connection guideline) - rename of some resistors
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/GitHub/N64RGB/advancedRGBmod/Main-PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Dropbox\blub\Main-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="159">
   <si>
     <t>Designator</t>
   </si>
@@ -35,9 +35,6 @@
     <t>R32</t>
   </si>
   <si>
-    <t>R10,R12,R13,R14,R15,R16,R17</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>8-LSSOP, 8-MSOP</t>
   </si>
   <si>
-    <t>www.digikey.de/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=234870828</t>
-  </si>
-  <si>
     <t>http://www.mouser.de/ProductDetail/Texas-Instruments/SN74LVC3G34DCTR/</t>
   </si>
   <si>
@@ -398,9 +392,6 @@
     <t>JTAG Connector</t>
   </si>
   <si>
-    <t>http://www.digikey.de/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=234877685</t>
-  </si>
-  <si>
     <t xml:space="preserve">RC0603FR-07536RL </t>
   </si>
   <si>
@@ -501,12 +492,24 @@
   </si>
   <si>
     <t>Cyclone 10 LP FPGA, 10k LE</t>
+  </si>
+  <si>
+    <t>R12,R13,R14,R15,R16</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/texas-instruments/SN74LVC3G34DCTR/296-13285-1-ND/484526</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/3m/30310-6002HB/30310-6002HB-ND/1237393</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/FkdFoXi5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1032,11 +1035,11 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1325,699 +1328,702 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
       <c r="G3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
         <v>55</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>63</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
         <v>119</v>
-      </c>
-      <c r="B17" t="s">
-        <v>121</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" t="s">
         <v>93</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>100</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>102</v>
-      </c>
       <c r="B20" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" t="s">
         <v>135</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" t="s">
-        <v>138</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
       <c r="B30" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2050,10 +2056,10 @@
     <hyperlink ref="I14" r:id="rId26"/>
     <hyperlink ref="I15" r:id="rId27"/>
     <hyperlink ref="H15" r:id="rId28"/>
-    <hyperlink ref="H18" r:id="rId29"/>
-    <hyperlink ref="I18" r:id="rId30"/>
-    <hyperlink ref="H19" r:id="rId31"/>
-    <hyperlink ref="I19" r:id="rId32"/>
+    <hyperlink ref="H19" r:id="rId29"/>
+    <hyperlink ref="I19" r:id="rId30"/>
+    <hyperlink ref="H18" r:id="rId31"/>
+    <hyperlink ref="I18" r:id="rId32"/>
     <hyperlink ref="H21" r:id="rId33"/>
     <hyperlink ref="I21" r:id="rId34"/>
     <hyperlink ref="I23" r:id="rId35"/>

</xml_diff>

<commit_message>
important BOM update: Use Schmitt triggered buffer instead of simple one!!!
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Dropbox\blub\Main-PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/GitHub/N64RGB/advancedRGBmod/Main-PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" refMode="R1C1"/>
+  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="158">
   <si>
     <t>Designator</t>
   </si>
@@ -80,9 +80,6 @@
     <t>U4</t>
   </si>
   <si>
-    <t>SN74LVC3G34DCTR</t>
-  </si>
-  <si>
     <t>http://www.digikey.de/short/3v93nm</t>
   </si>
   <si>
@@ -125,15 +122,9 @@
     <t>http://www.mouser.de/ProductDetail/STMicroelectronics/TSH122ICT/</t>
   </si>
   <si>
-    <t>Non-Inv Buffer 3Ch.</t>
-  </si>
-  <si>
     <t>8-LSSOP, 8-MSOP</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Texas-Instruments/SN74LVC3G34DCTR/</t>
-  </si>
-  <si>
     <t>SMD1206</t>
   </si>
   <si>
@@ -479,9 +470,6 @@
     <t xml:space="preserve">IC FLASH 16MBIT 108MHZ 8SOIC </t>
   </si>
   <si>
-    <t>TI: DCT Package Footprint, Alternative: 74HC3G34DP</t>
-  </si>
-  <si>
     <t>10CL010YE144C8G</t>
   </si>
   <si>
@@ -497,19 +485,28 @@
     <t>R12,R13,R14,R15,R16</t>
   </si>
   <si>
-    <t>https://www.digikey.de/product-detail/de/texas-instruments/SN74LVC3G34DCTR/296-13285-1-ND/484526</t>
-  </si>
-  <si>
     <t>https://www.digikey.de/product-detail/de/3m/30310-6002HB/30310-6002HB-ND/1237393</t>
   </si>
   <si>
-    <t>https://oshpark.com/shared_projects/FkdFoXi5</t>
+    <t>SN74LVC3G17DCTR</t>
+  </si>
+  <si>
+    <t>TI: DCT Package Footprint</t>
+  </si>
+  <si>
+    <t>http://www.mouser.de/ProductDetail/Texas-Instruments/SN74LVC3G17DCTR/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/texas-instruments/SN74LVC3G17DCTR/296-16915-1-ND/644203</t>
+  </si>
+  <si>
+    <t>Non-Inv Buffer 3Ch., Schmitt Trigger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1035,11 +1032,11 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1328,18 +1325,18 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1350,77 +1347,77 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
       <c r="G3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1431,174 +1428,174 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>153</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>157</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>156</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F7" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
         <v>52</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G9" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1607,50 +1604,50 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
         <v>69</v>
       </c>
-      <c r="F11" t="s">
-        <v>72</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1659,22 +1656,22 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1685,22 +1682,22 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1711,198 +1708,198 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
       <c r="D19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="I19" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1913,117 +1910,114 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F23" t="s">
-        <v>72</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" t="s">
         <v>132</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B26" t="s">
-        <v>135</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>158</v>
-      </c>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2034,49 +2028,48 @@
     <hyperlink ref="I3" r:id="rId4"/>
     <hyperlink ref="I4" r:id="rId5"/>
     <hyperlink ref="H4" r:id="rId6"/>
-    <hyperlink ref="H5" r:id="rId7"/>
-    <hyperlink ref="I5" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
-    <hyperlink ref="H10" r:id="rId10"/>
-    <hyperlink ref="H12" r:id="rId11"/>
-    <hyperlink ref="I12" r:id="rId12"/>
-    <hyperlink ref="I6" r:id="rId13"/>
-    <hyperlink ref="H7" r:id="rId14"/>
-    <hyperlink ref="I7" r:id="rId15"/>
-    <hyperlink ref="H8" r:id="rId16"/>
-    <hyperlink ref="I8" r:id="rId17"/>
-    <hyperlink ref="H9" r:id="rId18"/>
-    <hyperlink ref="I9" r:id="rId19"/>
-    <hyperlink ref="H11" r:id="rId20"/>
-    <hyperlink ref="I11" r:id="rId21"/>
-    <hyperlink ref="I13" r:id="rId22"/>
-    <hyperlink ref="H13" r:id="rId23"/>
-    <hyperlink ref="I16" r:id="rId24"/>
-    <hyperlink ref="H14" r:id="rId25"/>
-    <hyperlink ref="I14" r:id="rId26"/>
-    <hyperlink ref="I15" r:id="rId27"/>
-    <hyperlink ref="H15" r:id="rId28"/>
-    <hyperlink ref="H19" r:id="rId29"/>
-    <hyperlink ref="I19" r:id="rId30"/>
-    <hyperlink ref="H18" r:id="rId31"/>
-    <hyperlink ref="I18" r:id="rId32"/>
-    <hyperlink ref="H21" r:id="rId33"/>
-    <hyperlink ref="I21" r:id="rId34"/>
-    <hyperlink ref="I23" r:id="rId35"/>
-    <hyperlink ref="H23" r:id="rId36"/>
-    <hyperlink ref="I22" r:id="rId37"/>
-    <hyperlink ref="H22" r:id="rId38"/>
-    <hyperlink ref="H25" r:id="rId39"/>
-    <hyperlink ref="I25" r:id="rId40"/>
-    <hyperlink ref="I17" r:id="rId41"/>
-    <hyperlink ref="H17" r:id="rId42"/>
-    <hyperlink ref="H20" r:id="rId43"/>
-    <hyperlink ref="I24" r:id="rId44"/>
-    <hyperlink ref="H24" r:id="rId45"/>
-    <hyperlink ref="I26" r:id="rId46"/>
-    <hyperlink ref="H26" r:id="rId47"/>
-    <hyperlink ref="I20" r:id="rId48"/>
-    <hyperlink ref="H6" r:id="rId49"/>
+    <hyperlink ref="I5" r:id="rId7"/>
+    <hyperlink ref="I10" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H12" r:id="rId10"/>
+    <hyperlink ref="I12" r:id="rId11"/>
+    <hyperlink ref="I6" r:id="rId12"/>
+    <hyperlink ref="H7" r:id="rId13"/>
+    <hyperlink ref="I7" r:id="rId14"/>
+    <hyperlink ref="H8" r:id="rId15"/>
+    <hyperlink ref="I8" r:id="rId16"/>
+    <hyperlink ref="H9" r:id="rId17"/>
+    <hyperlink ref="I9" r:id="rId18"/>
+    <hyperlink ref="H11" r:id="rId19"/>
+    <hyperlink ref="I11" r:id="rId20"/>
+    <hyperlink ref="I13" r:id="rId21"/>
+    <hyperlink ref="H13" r:id="rId22"/>
+    <hyperlink ref="I16" r:id="rId23"/>
+    <hyperlink ref="H14" r:id="rId24"/>
+    <hyperlink ref="I14" r:id="rId25"/>
+    <hyperlink ref="I15" r:id="rId26"/>
+    <hyperlink ref="H15" r:id="rId27"/>
+    <hyperlink ref="H19" r:id="rId28"/>
+    <hyperlink ref="I19" r:id="rId29"/>
+    <hyperlink ref="H18" r:id="rId30"/>
+    <hyperlink ref="I18" r:id="rId31"/>
+    <hyperlink ref="H21" r:id="rId32"/>
+    <hyperlink ref="I21" r:id="rId33"/>
+    <hyperlink ref="I23" r:id="rId34"/>
+    <hyperlink ref="H23" r:id="rId35"/>
+    <hyperlink ref="I22" r:id="rId36"/>
+    <hyperlink ref="H22" r:id="rId37"/>
+    <hyperlink ref="H25" r:id="rId38"/>
+    <hyperlink ref="I25" r:id="rId39"/>
+    <hyperlink ref="I17" r:id="rId40"/>
+    <hyperlink ref="H17" r:id="rId41"/>
+    <hyperlink ref="H20" r:id="rId42"/>
+    <hyperlink ref="I24" r:id="rId43"/>
+    <hyperlink ref="H24" r:id="rId44"/>
+    <hyperlink ref="I26" r:id="rId45"/>
+    <hyperlink ref="H26" r:id="rId46"/>
+    <hyperlink ref="I20" r:id="rId47"/>
+    <hyperlink ref="H6" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PCB - reroute power supply layer reducing noise injection to +5V plane from digital signals - adapt some component positions
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/GitHub/N64RGB/advancedRGBmod/Main-PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Dropbox/blub/Main-PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="157">
   <si>
     <t>Designator</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>U4</t>
-  </si>
-  <si>
-    <t>http://www.digikey.de/short/3v93nm</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
@@ -993,13 +990,14 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1322,11 +1320,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1336,33 +1332,33 @@
     <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1370,25 +1366,25 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1396,25 +1392,25 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
       <c r="G3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1428,16 +1424,16 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1445,157 +1441,157 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
         <v>57</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>58</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1604,50 +1600,50 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
         <v>65</v>
       </c>
-      <c r="E11" t="s">
-        <v>66</v>
-      </c>
       <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1656,19 +1652,19 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1682,19 +1678,19 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1708,62 +1704,62 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
         <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>77</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1771,132 +1767,132 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
       <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" t="s">
         <v>88</v>
       </c>
-      <c r="E19" t="s">
-        <v>89</v>
-      </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
         <v>119</v>
       </c>
-      <c r="F20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="I20" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F21" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1910,103 +1906,103 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2014,11 +2010,6 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add missing ceramic cap
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Dropbox/blub/Main-PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/GitHub/N64RGB/advancedRGBmod/Main-PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
   <si>
     <t>Designator</t>
   </si>
@@ -498,6 +498,21 @@
   </si>
   <si>
     <t>Non-Inv Buffer 3Ch., Schmitt Trigger</t>
+  </si>
+  <si>
+    <t>C601,C602,C701,C702</t>
+  </si>
+  <si>
+    <t>GRM18R60J105KA01J</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/murata-electronics-north-america/GRM188R60J105KA01J/490-6404-1-ND/3845601</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Murata/GRM188R60J105KA01J/</t>
+  </si>
+  <si>
+    <t>1uF / 6.3V</t>
   </si>
 </sst>
 </file>
@@ -1320,9 +1335,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1721,186 +1738,186 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>161</v>
       </c>
       <c r="F16" t="s">
         <v>68</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>78</v>
+        <v>159</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>79</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" t="s">
-        <v>68</v>
+      <c r="G18" t="s">
+        <v>116</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>150</v>
-      </c>
-      <c r="B19" t="s">
-        <v>91</v>
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
         <v>68</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>117</v>
+        <v>150</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>118</v>
+      <c r="E20" t="s">
+        <v>88</v>
       </c>
       <c r="F20" t="s">
         <v>68</v>
       </c>
-      <c r="G20" t="s">
-        <v>119</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>87</v>
       </c>
-      <c r="E21" t="s">
-        <v>97</v>
+      <c r="E21" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="F21" t="s">
         <v>68</v>
       </c>
+      <c r="G21" t="s">
+        <v>119</v>
+      </c>
       <c r="H21" s="1" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
+        <v>110</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>102</v>
+      <c r="E22" t="s">
+        <v>97</v>
       </c>
       <c r="F22" t="s">
         <v>68</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1909,24 +1926,24 @@
         <v>87</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F23" t="s">
         <v>68</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1935,81 +1952,107 @@
         <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F24" t="s">
         <v>68</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>127</v>
+        <v>68</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
         <v>108</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F26" t="s">
         <v>31</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2035,31 +2078,31 @@
     <hyperlink ref="I11" r:id="rId20"/>
     <hyperlink ref="I13" r:id="rId21"/>
     <hyperlink ref="H13" r:id="rId22"/>
-    <hyperlink ref="I16" r:id="rId23"/>
+    <hyperlink ref="I17" r:id="rId23"/>
     <hyperlink ref="H14" r:id="rId24"/>
     <hyperlink ref="I14" r:id="rId25"/>
     <hyperlink ref="I15" r:id="rId26"/>
     <hyperlink ref="H15" r:id="rId27"/>
-    <hyperlink ref="H19" r:id="rId28"/>
-    <hyperlink ref="I19" r:id="rId29"/>
-    <hyperlink ref="H18" r:id="rId30"/>
-    <hyperlink ref="I18" r:id="rId31"/>
-    <hyperlink ref="H21" r:id="rId32"/>
-    <hyperlink ref="I21" r:id="rId33"/>
-    <hyperlink ref="I23" r:id="rId34"/>
-    <hyperlink ref="H23" r:id="rId35"/>
-    <hyperlink ref="I22" r:id="rId36"/>
-    <hyperlink ref="H22" r:id="rId37"/>
-    <hyperlink ref="H25" r:id="rId38"/>
-    <hyperlink ref="I25" r:id="rId39"/>
-    <hyperlink ref="I17" r:id="rId40"/>
-    <hyperlink ref="H17" r:id="rId41"/>
-    <hyperlink ref="H20" r:id="rId42"/>
-    <hyperlink ref="I24" r:id="rId43"/>
-    <hyperlink ref="H24" r:id="rId44"/>
-    <hyperlink ref="I26" r:id="rId45"/>
-    <hyperlink ref="H26" r:id="rId46"/>
-    <hyperlink ref="I20" r:id="rId47"/>
+    <hyperlink ref="H20" r:id="rId28"/>
+    <hyperlink ref="I20" r:id="rId29"/>
+    <hyperlink ref="H19" r:id="rId30"/>
+    <hyperlink ref="I19" r:id="rId31"/>
+    <hyperlink ref="H22" r:id="rId32"/>
+    <hyperlink ref="I22" r:id="rId33"/>
+    <hyperlink ref="I24" r:id="rId34"/>
+    <hyperlink ref="H24" r:id="rId35"/>
+    <hyperlink ref="I23" r:id="rId36"/>
+    <hyperlink ref="H23" r:id="rId37"/>
+    <hyperlink ref="H26" r:id="rId38"/>
+    <hyperlink ref="I26" r:id="rId39"/>
+    <hyperlink ref="I18" r:id="rId40"/>
+    <hyperlink ref="H18" r:id="rId41"/>
+    <hyperlink ref="H21" r:id="rId42"/>
+    <hyperlink ref="I25" r:id="rId43"/>
+    <hyperlink ref="H25" r:id="rId44"/>
+    <hyperlink ref="I27" r:id="rId45"/>
+    <hyperlink ref="H27" r:id="rId46"/>
+    <hyperlink ref="I21" r:id="rId47"/>
     <hyperlink ref="H6" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add missing caps in BOM
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Dropbox/blub/Main-PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/GitHub/N64RGB/advancedRGBmod/Main-PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
   <si>
     <t>Designator</t>
   </si>
@@ -498,6 +498,21 @@
   </si>
   <si>
     <t>Non-Inv Buffer 3Ch., Schmitt Trigger</t>
+  </si>
+  <si>
+    <t>C601,C602,C701,C702</t>
+  </si>
+  <si>
+    <t>GRM18R60J105KA01J</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/murata-electronics-north-america/GRM188R60J105KA01J/490-6404-1-ND/3845601</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Murata/GRM188R60J105KA01J/</t>
+  </si>
+  <si>
+    <t>1uF / 6.3V</t>
   </si>
 </sst>
 </file>
@@ -1320,9 +1335,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1721,186 +1738,186 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>161</v>
       </c>
       <c r="F16" t="s">
         <v>68</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>78</v>
+        <v>159</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>79</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" t="s">
-        <v>68</v>
+      <c r="G18" t="s">
+        <v>116</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>150</v>
-      </c>
-      <c r="B19" t="s">
-        <v>91</v>
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
         <v>68</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>117</v>
+        <v>150</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>118</v>
+      <c r="E20" t="s">
+        <v>88</v>
       </c>
       <c r="F20" t="s">
         <v>68</v>
       </c>
-      <c r="G20" t="s">
-        <v>119</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>87</v>
       </c>
-      <c r="E21" t="s">
-        <v>97</v>
+      <c r="E21" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="F21" t="s">
         <v>68</v>
       </c>
+      <c r="G21" t="s">
+        <v>119</v>
+      </c>
       <c r="H21" s="1" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
+        <v>110</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>102</v>
+      <c r="E22" t="s">
+        <v>97</v>
       </c>
       <c r="F22" t="s">
         <v>68</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1909,24 +1926,24 @@
         <v>87</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F23" t="s">
         <v>68</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1935,81 +1952,107 @@
         <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F24" t="s">
         <v>68</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>127</v>
+        <v>68</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
         <v>108</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F26" t="s">
         <v>31</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2035,31 +2078,31 @@
     <hyperlink ref="I11" r:id="rId20"/>
     <hyperlink ref="I13" r:id="rId21"/>
     <hyperlink ref="H13" r:id="rId22"/>
-    <hyperlink ref="I16" r:id="rId23"/>
+    <hyperlink ref="I17" r:id="rId23"/>
     <hyperlink ref="H14" r:id="rId24"/>
     <hyperlink ref="I14" r:id="rId25"/>
     <hyperlink ref="I15" r:id="rId26"/>
     <hyperlink ref="H15" r:id="rId27"/>
-    <hyperlink ref="H19" r:id="rId28"/>
-    <hyperlink ref="I19" r:id="rId29"/>
-    <hyperlink ref="H18" r:id="rId30"/>
-    <hyperlink ref="I18" r:id="rId31"/>
-    <hyperlink ref="H21" r:id="rId32"/>
-    <hyperlink ref="I21" r:id="rId33"/>
-    <hyperlink ref="I23" r:id="rId34"/>
-    <hyperlink ref="H23" r:id="rId35"/>
-    <hyperlink ref="I22" r:id="rId36"/>
-    <hyperlink ref="H22" r:id="rId37"/>
-    <hyperlink ref="H25" r:id="rId38"/>
-    <hyperlink ref="I25" r:id="rId39"/>
-    <hyperlink ref="I17" r:id="rId40"/>
-    <hyperlink ref="H17" r:id="rId41"/>
-    <hyperlink ref="H20" r:id="rId42"/>
-    <hyperlink ref="I24" r:id="rId43"/>
-    <hyperlink ref="H24" r:id="rId44"/>
-    <hyperlink ref="I26" r:id="rId45"/>
-    <hyperlink ref="H26" r:id="rId46"/>
-    <hyperlink ref="I20" r:id="rId47"/>
+    <hyperlink ref="H20" r:id="rId28"/>
+    <hyperlink ref="I20" r:id="rId29"/>
+    <hyperlink ref="H19" r:id="rId30"/>
+    <hyperlink ref="I19" r:id="rId31"/>
+    <hyperlink ref="H22" r:id="rId32"/>
+    <hyperlink ref="I22" r:id="rId33"/>
+    <hyperlink ref="I24" r:id="rId34"/>
+    <hyperlink ref="H24" r:id="rId35"/>
+    <hyperlink ref="I23" r:id="rId36"/>
+    <hyperlink ref="H23" r:id="rId37"/>
+    <hyperlink ref="H26" r:id="rId38"/>
+    <hyperlink ref="I26" r:id="rId39"/>
+    <hyperlink ref="I18" r:id="rId40"/>
+    <hyperlink ref="H18" r:id="rId41"/>
+    <hyperlink ref="H21" r:id="rId42"/>
+    <hyperlink ref="I25" r:id="rId43"/>
+    <hyperlink ref="H25" r:id="rId44"/>
+    <hyperlink ref="I27" r:id="rId45"/>
+    <hyperlink ref="H27" r:id="rId46"/>
+    <hyperlink ref="I21" r:id="rId47"/>
     <hyperlink ref="H6" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add TOP, BOT and THT pages in BOM
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -13,6 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
+    <sheet name="TOP" sheetId="5" r:id="rId2"/>
+    <sheet name="BOT" sheetId="6" r:id="rId3"/>
+    <sheet name="THT" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="170">
   <si>
     <t>Designator</t>
   </si>
@@ -513,6 +516,30 @@
   </si>
   <si>
     <t>1uF / 6.3V</t>
+  </si>
+  <si>
+    <t>C121,C301</t>
+  </si>
+  <si>
+    <t>C101</t>
+  </si>
+  <si>
+    <t>C202,C204,C206</t>
+  </si>
+  <si>
+    <t>C302,C801</t>
+  </si>
+  <si>
+    <t>R14,R15,R16</t>
+  </si>
+  <si>
+    <t>R12,R13</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R22,R52,R53</t>
   </si>
 </sst>
 </file>
@@ -1337,9 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1914,10 +1939,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1926,24 +1951,24 @@
         <v>87</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" t="s">
         <v>68</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1952,16 +1977,16 @@
         <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
         <v>68</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -2089,10 +2114,10 @@
     <hyperlink ref="I19" r:id="rId31"/>
     <hyperlink ref="H22" r:id="rId32"/>
     <hyperlink ref="I22" r:id="rId33"/>
-    <hyperlink ref="I24" r:id="rId34"/>
-    <hyperlink ref="H24" r:id="rId35"/>
-    <hyperlink ref="I23" r:id="rId36"/>
-    <hyperlink ref="H23" r:id="rId37"/>
+    <hyperlink ref="I23" r:id="rId34"/>
+    <hyperlink ref="H23" r:id="rId35"/>
+    <hyperlink ref="I24" r:id="rId36"/>
+    <hyperlink ref="H24" r:id="rId37"/>
     <hyperlink ref="H26" r:id="rId38"/>
     <hyperlink ref="I26" r:id="rId39"/>
     <hyperlink ref="I18" r:id="rId40"/>
@@ -2107,4 +2132,849 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bugfix (forget to change MPN of R21 on last change)
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="171">
   <si>
     <t>Designator</t>
   </si>
@@ -540,6 +540,9 @@
   </si>
   <si>
     <t>https://www.digikey.de/product-detail/de/yageo/RC0603FR-07523RL/311-523HRCT-ND/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-07523RL </t>
   </si>
 </sst>
 </file>
@@ -1364,7 +1367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1887,7 +1892,7 @@
         <v>96</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>117</v>
+        <v>170</v>
       </c>
       <c r="C21">
         <v>1</v>

</xml_diff>

<commit_message>
Place R21 (R_set of the DAC) on TOP layer making it easy to replace if board is installed
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
+++ b/advancedRGBmod/Main-PCB/BOM_n64advanced.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/Git/N64RGB/advancedRGBmod/Main-PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Documents\Workspaces\Git\n64rgb\advancedRGBmod\Main-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="170">
   <si>
     <t>Designator</t>
   </si>
@@ -381,9 +381,6 @@
   </si>
   <si>
     <t>JTAG Connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-07536RL </t>
   </si>
   <si>
     <t>RC0603FR-0724R9L</t>
@@ -548,7 +545,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1075,11 +1072,11 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1367,19 +1364,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1408,18 +1403,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -1428,18 +1423,18 @@
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1451,16 +1446,16 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1483,59 +1478,59 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F5" t="s">
         <v>30</v>
       </c>
       <c r="G5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1558,7 +1553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1581,7 +1576,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1610,7 +1605,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1636,7 +1631,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -1662,12 +1657,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -1688,7 +1683,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1714,7 +1709,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1735,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1766,12 +1761,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" t="s">
         <v>153</v>
-      </c>
-      <c r="B16" t="s">
-        <v>154</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1780,19 +1775,19 @@
         <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F16" t="s">
         <v>68</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -1815,7 +1810,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>113</v>
       </c>
@@ -1829,13 +1824,13 @@
         <v>116</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1861,9 +1856,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
         <v>91</v>
@@ -1887,12 +1882,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>96</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1901,22 +1896,22 @@
         <v>87</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F21" t="s">
         <v>68</v>
       </c>
       <c r="G21" t="s">
+        <v>167</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="I21" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>110</v>
       </c>
@@ -1942,7 +1937,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1968,9 +1963,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
         <v>103</v>
@@ -1994,12 +1989,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2014,18 +2009,18 @@
         <v>68</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -2040,21 +2035,21 @@
         <v>31</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -2069,19 +2064,19 @@
         <v>31</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
   </sheetData>
@@ -2141,19 +2136,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2176,18 +2171,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -2198,12 +2193,12 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2215,12 +2210,12 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2239,29 +2234,29 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F5" t="s">
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2280,7 +2275,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2299,7 +2294,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2324,7 +2319,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -2346,12 +2341,12 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2368,9 +2363,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -2390,7 +2385,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2412,7 +2407,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2434,12 +2429,12 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" t="s">
         <v>153</v>
-      </c>
-      <c r="B14" t="s">
-        <v>154</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -2448,7 +2443,7 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F14" t="s">
         <v>68</v>
@@ -2456,7 +2451,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -2475,9 +2470,9 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" t="s">
         <v>91</v>
@@ -2497,12 +2492,12 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2510,21 +2505,24 @@
       <c r="D17" t="s">
         <v>87</v>
       </c>
-      <c r="E17" t="s">
-        <v>97</v>
+      <c r="E17" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="F17" t="s">
         <v>68</v>
       </c>
+      <c r="G17" t="s">
+        <v>167</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
+        <v>163</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2532,8 +2530,8 @@
       <c r="D18" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>101</v>
+      <c r="E18" t="s">
+        <v>97</v>
       </c>
       <c r="F18" t="s">
         <v>68</v>
@@ -2541,12 +2539,12 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2555,7 +2553,7 @@
         <v>87</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F19" t="s">
         <v>68</v>
@@ -2563,61 +2561,83 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
         <v>108</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
         <v>31</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2626,19 +2646,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2661,29 +2681,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -2705,12 +2725,12 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2727,9 +2747,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2749,7 +2769,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2771,9 +2791,9 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
         <v>91</v>
@@ -2793,46 +2813,43 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>164</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>166</v>
+      <c r="E8" t="s">
+        <v>97</v>
       </c>
       <c r="F8" t="s">
         <v>68</v>
       </c>
-      <c r="G8" t="s">
-        <v>168</v>
-      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>100</v>
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>87</v>
       </c>
-      <c r="E9" t="s">
-        <v>97</v>
+      <c r="E9" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
@@ -2840,33 +2857,11 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2879,15 +2874,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2910,7 +2905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -2926,57 +2921,57 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" s="3"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="4"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="4"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
   </sheetData>

</xml_diff>